<commit_message>
Ajuste local de salvamento
</commit_message>
<xml_diff>
--- a/censo_internados.xlsx
+++ b/censo_internados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,13 +436,13 @@
     <col width="4" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
     <col width="9" customWidth="1" min="3" max="3"/>
-    <col width="24" customWidth="1" min="4" max="4"/>
+    <col width="29" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
     <col width="22" customWidth="1" min="6" max="6"/>
     <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="18" customWidth="1" min="8" max="8"/>
-    <col width="14" customWidth="1" min="9" max="9"/>
-    <col width="35" customWidth="1" min="10" max="10"/>
+    <col width="33" customWidth="1" min="8" max="8"/>
+    <col width="29" customWidth="1" min="9" max="9"/>
+    <col width="22" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -515,7 +515,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NILZA MARTINHO RICARDO</t>
+          <t>Beneficiário não encontrado</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -535,17 +535,17 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>03/02/25</t>
+          <t>Data de admissão não encontrada</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>06/02/25</t>
+          <t>Data de alta não encontrada</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Insuficiência cardíaca congestiva</t>
+          <t>MOTIVO NÃO INFORMADO</t>
         </is>
       </c>
     </row>
@@ -567,7 +567,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>NILZA MARTINHO RICARDO</t>
+          <t>Beneficiário não encontrado</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -587,121 +587,17 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>03/02/25</t>
+          <t>Data de admissão não encontrada</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>06/02/25</t>
+          <t>Data de alta não encontrada</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Insuficiência cardíaca congestiva</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>SC</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>CLINICA</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ELETIVO</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>NILZA MARTINHO RICARDO</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>APARTAMENTO</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>UNIMED FLORIANOPOLIS</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>77.658.611/0001-08</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>03/02/25</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>06/02/25</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Insuficiência cardíaca congestiva</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>SC</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>CLINICA</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>ELETIVO</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>NILZA MARTINHO RICARDO</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>APARTAMENTO</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>UNIMED FLORIANOPOLIS</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>77.658.611/0001-08</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>03/02/25</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>06/02/25</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Insuficiência cardíaca congestiva</t>
+          <t>MOTIVO NÃO INFORMADO</t>
         </is>
       </c>
     </row>

</xml_diff>